<commit_message>
Update Custom Expression CF sample
</commit_message>
<xml_diff>
--- a/SamplesLibrary.Engine/Files/Engine/CustomExpressionSampleData.xlsx
+++ b/SamplesLibrary.Engine/Files/Engine/CustomExpressionSampleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\_projects\SpreadsheetGearExplorer\SharedEngineSampleCode\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\_projects\SpreadsheetGearExplorerSamples\SamplesLibrary.Engine\Files\Engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEA6597-8582-4F53-9245-1C0A3592C2FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5B7629-25C9-4BA2-B0BE-9189D8991DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16650" yWindow="2660" windowWidth="24410" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>.NET Framework 1.0</t>
   </si>
@@ -41,30 +41,18 @@
     <t>January 15, 2002</t>
   </si>
   <si>
-    <t>October 17, 2013</t>
-  </si>
-  <si>
     <t>July 20, 2015</t>
   </si>
   <si>
     <t>April 5, 2017</t>
   </si>
   <si>
-    <t>October 17, 2017</t>
-  </si>
-  <si>
     <t>.NET Core 2.1</t>
   </si>
   <si>
     <t>.NET Framework 4.6</t>
   </si>
   <si>
-    <t>.NET Framework 4.5.1</t>
-  </si>
-  <si>
-    <t>.NET Framework 4.7.1</t>
-  </si>
-  <si>
     <t>.NET Version</t>
   </si>
   <si>
@@ -95,18 +83,6 @@
     <t>November 6, 2006</t>
   </si>
   <si>
-    <t>November 30, 2015</t>
-  </si>
-  <si>
-    <t>April 30, 2018</t>
-  </si>
-  <si>
-    <t>.NET Framework 4.5.2</t>
-  </si>
-  <si>
-    <t>.NET Framework 4.7.2</t>
-  </si>
-  <si>
     <t>December 3, 2019</t>
   </si>
   <si>
@@ -146,15 +122,9 @@
     <t>Release Date</t>
   </si>
   <si>
-    <t>.NET Framework 4.6.1</t>
-  </si>
-  <si>
     <t>.NET Framework 4.5</t>
   </si>
   <si>
-    <t>August 2, 2016</t>
-  </si>
-  <si>
     <t>December 4, 2018</t>
   </si>
   <si>
@@ -170,16 +140,22 @@
     <t>April 18, 2019</t>
   </si>
   <si>
-    <t>.NET Framework 4.6.2</t>
-  </si>
-  <si>
-    <t>May 5, 2014</t>
-  </si>
-  <si>
     <t>.NET 5</t>
   </si>
   <si>
     <t>November 10, 2020</t>
+  </si>
+  <si>
+    <t>.NET 6</t>
+  </si>
+  <si>
+    <t>.NET 7</t>
+  </si>
+  <si>
+    <t>November 8, 2021</t>
+  </si>
+  <si>
+    <t>November 8, 2022</t>
   </si>
 </sst>
 </file>
@@ -557,27 +533,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.17578125" customWidth="1"/>
-    <col min="2" max="2" width="19.87890625" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" customWidth="1"/>
+    <col min="2" max="2" width="19.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,188 +561,156 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A12" s="1" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>